<commit_message>
we may have a winner
</commit_message>
<xml_diff>
--- a/Spreadsheet-ACI-backup.xlsx
+++ b/Spreadsheet-ACI-backup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28DC9F0-7D05-4113-86FA-3B225204DD61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED56B295-6485-4C93-8E60-BED00994EC41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="15" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3241" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3241" uniqueCount="1158">
   <si>
     <t>Type</t>
   </si>
@@ -4290,6 +4290,9 @@
   </si>
   <si>
     <t>enable</t>
+  </si>
+  <si>
+    <t>Once Again Changed</t>
   </si>
 </sst>
 </file>
@@ -6048,8 +6051,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6204,7 +6207,7 @@
         <v>298</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>299</v>
+        <v>1157</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>475</v>
@@ -8700,8 +8703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AG141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE22" sqref="AE22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15852,7 +15855,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z76"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
@@ -18217,7 +18220,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -22527,7 +22530,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>

</xml_diff>